<commit_message>
got main expenes and living expenses in there
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke.ruane/Documents/GitHub/Budgeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F52E9EC-D161-9A4E-A305-7392251FD572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1BC6FA-2133-1A4B-807A-33FFD5BDA332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" firstSheet="1" activeTab="1" xr2:uid="{917D1629-3A58-1142-9852-AF8D807584E0}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{917D1629-3A58-1142-9852-AF8D807584E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Savings &amp; Investments" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304639FC-9708-4047-B383-41C782CD4280}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D2373B-2157-3E45-83EE-E971CAB6AE19}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>